<commit_message>
used functions(though it got bigger)
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taa\Desktop\PythonProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8FC81A-78E4-4522-8F3E-EA0163723702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F40C2FA-2C8E-4ED8-8A08-A18FD8EA6CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -52,6 +52,15 @@
     <t>Events</t>
   </si>
   <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Reg Number</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
     <t>Tafadzwa</t>
   </si>
   <si>
@@ -64,18 +73,111 @@
     <t>male</t>
   </si>
   <si>
+    <t>765xc00</t>
+  </si>
+  <si>
+    <t>R241273X</t>
+  </si>
+  <si>
+    <t>Bleightjbande@gmail.com</t>
+  </si>
+  <si>
+    <t>Brandon</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-04-16 </t>
+  </si>
+  <si>
+    <t>23:08</t>
+  </si>
+  <si>
+    <t>843ac90</t>
+  </si>
+  <si>
+    <t>Brandonbande01@gmail.com</t>
+  </si>
+  <si>
+    <t>Tanaka</t>
+  </si>
+  <si>
+    <t>Boiz</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>23:06</t>
+  </si>
+  <si>
+    <t>765xc5</t>
+  </si>
+  <si>
+    <t>Tanakaboys100@gmail.com</t>
+  </si>
+  <si>
+    <t>Wadzanai</t>
+  </si>
+  <si>
+    <t>Chadambuka</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>25-04-17</t>
+  </si>
+  <si>
+    <t>01:39</t>
+  </si>
+  <si>
+    <t>081gs493</t>
+  </si>
+  <si>
+    <t>Belinda</t>
+  </si>
+  <si>
+    <t>Choruwa</t>
+  </si>
+  <si>
+    <t>489dy888</t>
+  </si>
+  <si>
+    <t>Belindahchoruwa@gmail.com</t>
+  </si>
+  <si>
+    <t>Chido</t>
+  </si>
+  <si>
+    <t>Makandigona</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>692hf78</t>
+  </si>
+  <si>
     <t xml:space="preserve">Panashe </t>
   </si>
   <si>
     <t>Mashava</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>678hg56</t>
   </si>
   <si>
+    <t>Panashemashava14141@gmail.com</t>
+  </si>
+  <si>
     <t>Praise</t>
   </si>
   <si>
@@ -85,97 +187,79 @@
     <t>100+</t>
   </si>
   <si>
-    <t xml:space="preserve">25-04-16 </t>
-  </si>
-  <si>
     <t>22:46</t>
   </si>
   <si>
     <t>764he23</t>
   </si>
   <si>
+    <t>Tanyaradzwa</t>
+  </si>
+  <si>
+    <t>Mudzengerere</t>
+  </si>
+  <si>
+    <t>00:32</t>
+  </si>
+  <si>
+    <t>567h190</t>
+  </si>
+  <si>
+    <t>Tanyamudzengerere@gmail.com</t>
+  </si>
+  <si>
+    <t>Trevor</t>
+  </si>
+  <si>
+    <t>Muvirimi</t>
+  </si>
+  <si>
+    <t>25-04-18</t>
+  </si>
+  <si>
+    <t>23:48</t>
+  </si>
+  <si>
+    <t>963ln745</t>
+  </si>
+  <si>
+    <t>Antony</t>
+  </si>
+  <si>
+    <t>Ndebvu</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>23:07</t>
+  </si>
+  <si>
+    <t>672vn81</t>
+  </si>
+  <si>
     <t>Ropafadzo</t>
   </si>
   <si>
     <t>Nyagura</t>
   </si>
   <si>
-    <t>Blue</t>
-  </si>
-  <si>
     <t>23:05</t>
   </si>
   <si>
     <t>289hg28</t>
   </si>
   <si>
-    <t>Chido</t>
-  </si>
-  <si>
-    <t>Makandigona</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>23:06</t>
-  </si>
-  <si>
-    <t>692hf78</t>
-  </si>
-  <si>
-    <t>Tanaka</t>
-  </si>
-  <si>
-    <t>Boiz</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>765xc5</t>
-  </si>
-  <si>
-    <t>Antony</t>
-  </si>
-  <si>
-    <t>Ndebvu</t>
-  </si>
-  <si>
-    <t>orange</t>
-  </si>
-  <si>
-    <t>23:07</t>
-  </si>
-  <si>
-    <t>672vn81</t>
-  </si>
-  <si>
-    <t>Brandon</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>23:08</t>
-  </si>
-  <si>
-    <t>843ac90</t>
-  </si>
-  <si>
-    <t>Tanyaradzwa</t>
-  </si>
-  <si>
-    <t>25-04-17</t>
-  </si>
-  <si>
-    <t>00:32</t>
-  </si>
-  <si>
-    <t>567h190</t>
+    <t>Ruvarashe</t>
+  </si>
+  <si>
+    <t>Shumba</t>
+  </si>
+  <si>
+    <t>22:41</t>
+  </si>
+  <si>
+    <t>065hb481</t>
   </si>
   <si>
     <t>Courage</t>
@@ -190,31 +274,76 @@
     <t>791oh631</t>
   </si>
   <si>
-    <t>Wadzanai</t>
-  </si>
-  <si>
-    <t>Chadambuka</t>
-  </si>
-  <si>
-    <t>01:39</t>
-  </si>
-  <si>
-    <t>081gs493</t>
-  </si>
-  <si>
-    <t>Belinda</t>
-  </si>
-  <si>
-    <t>Choruwa</t>
-  </si>
-  <si>
-    <t>489dy888</t>
-  </si>
-  <si>
-    <t>Mudzengerere</t>
-  </si>
-  <si>
-    <t>765xc00</t>
+    <t>cherrychosa@gmail.com</t>
+  </si>
+  <si>
+    <t>Charity</t>
+  </si>
+  <si>
+    <t>Chosa</t>
+  </si>
+  <si>
+    <t>25-04-19</t>
+  </si>
+  <si>
+    <t>00:23</t>
+  </si>
+  <si>
+    <t>321xd991</t>
+  </si>
+  <si>
+    <t>Rachiel</t>
+  </si>
+  <si>
+    <t>Chimbudzi</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>00:29</t>
+  </si>
+  <si>
+    <t>037za435</t>
+  </si>
+  <si>
+    <t>+27812525147</t>
+  </si>
+  <si>
+    <t>+447823961094</t>
+  </si>
+  <si>
+    <t>0776688563</t>
+  </si>
+  <si>
+    <t>0779498932</t>
+  </si>
+  <si>
+    <t>0784891744</t>
+  </si>
+  <si>
+    <t>0773292910</t>
+  </si>
+  <si>
+    <t>0712542901</t>
+  </si>
+  <si>
+    <t>0787205939</t>
+  </si>
+  <si>
+    <t>0780828900</t>
+  </si>
+  <si>
+    <t>0780935065</t>
+  </si>
+  <si>
+    <t>0785251040</t>
+  </si>
+  <si>
+    <t>0777237673</t>
+  </si>
+  <si>
+    <t>Sky Blue</t>
   </si>
 </sst>
 </file>
@@ -270,11 +399,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,21 +711,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,13 +765,22 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>25</v>
@@ -637,242 +789,260 @@
         <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
       <c r="C3">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D3">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C4">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>27</v>
+      </c>
+      <c r="D5">
         <v>23</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>25</v>
-      </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C6">
         <v>25</v>
       </c>
       <c r="D6">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
         <v>45</v>
       </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
       <c r="C7">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8">
-        <v>22</v>
-      </c>
-      <c r="D8">
+      <c r="I8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>27</v>
-      </c>
-      <c r="D9">
-        <v>67</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="I9" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C10">
         <v>24</v>
@@ -881,121 +1051,262 @@
         <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="M10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C11">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D11">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C12">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D12">
         <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="H12" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="I12" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="J12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
         <v>25</v>
       </c>
-      <c r="D13">
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" t="s">
+        <v>75</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I15" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16">
+        <v>27</v>
+      </c>
+      <c r="D16">
         <v>98</v>
       </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="M16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17">
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <v>64</v>
+      </c>
+      <c r="E17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" t="s">
+        <v>94</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="K10 K16" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>